<commit_message>
child allowance is only paid for "kindergeld-Kinder". kindergeld eligibility is sourced out to 'tb' dictionary. kindergeld test is corrected
Former-commit-id: b2c68981c69c4b90c5b960d54e8b2c8f14ad40e2
Former-commit-id: 264c0a2a585f54215853c7d71bf072f0d78b9baf
</commit_message>
<xml_diff>
--- a/tests/test_tax_transfers/test_data/test_dfs_zve.xlsx
+++ b/tests/test_tax_transfers/test_data/test_dfs_zve.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>tu_id</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>pid</t>
+  </si>
+  <si>
+    <t>w_hours</t>
+  </si>
+  <si>
+    <t>ineducation</t>
   </si>
 </sst>
 </file>
@@ -474,20 +480,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ30"/>
+  <dimension ref="A1:AL30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="12" width="13.7109375" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" style="1"/>
+    <col min="13" max="14" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -513,82 +519,88 @@
         <v>9</v>
       </c>
       <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>2</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>4</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>3</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>14</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>17</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>B2</f>
         <v>1</v>
@@ -612,28 +624,29 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H19" si="0">U2+(65-S2)</f>
+        <f t="shared" ref="H2:H19" si="0">W2+(65-U2)</f>
         <v>2043</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <f>(N2=FALSE)*40+(N2=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K2" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K2">
         <v>0</v>
       </c>
       <c r="L2" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
+      <c r="M2" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="O2">
@@ -645,52 +658,58 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2" t="b">
-        <f>FALSE</f>
+      <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>40</v>
-      </c>
-      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="T2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="U2">
+        <v>40</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
         <v>2018</v>
       </c>
-      <c r="V2" s="2">
-        <f t="shared" ref="V2:V13" si="1">MAX(AB2-AA2-36,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W2" s="2">
-        <f t="shared" ref="W2:W14" si="2">V2-AC2</f>
-        <v>0</v>
-      </c>
-      <c r="X2" s="1">
-        <f>V2+MAX(F2*12-801-36,0)</f>
+      <c r="X2" s="2">
+        <f t="shared" ref="X2:X13" si="1">MAX(AD2-AC2-36,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y2" s="2">
+        <f t="shared" ref="Y2:Y14" si="2">X2-AE2</f>
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1">
+        <f>X2+MAX(F2*12-801-36,0)</f>
         <v>363</v>
       </c>
-      <c r="Y2" s="1">
-        <f>MAX(X2-AC3,0)</f>
+      <c r="AA2" s="1">
+        <f>MAX(Z2-AE3,0)</f>
         <v>363</v>
       </c>
-      <c r="AA2">
-        <f t="shared" ref="AA2:AA12" si="3">INT(((0.6+(0.02*(U2-2005)))*(2*12*N2))-(12*N2))+AD2</f>
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <f t="shared" ref="AB2:AB7" si="4">(12*E2+(12*D2 - 1000)*(D2&gt;450))</f>
-        <v>0</v>
-      </c>
       <c r="AC2">
+        <f t="shared" ref="AC2:AC12" si="3">INT(((0.6+(0.02*(W2-2005)))*(2*12*P2))-(12*P2))+AF2</f>
         <v>0</v>
       </c>
       <c r="AD2">
-        <f t="shared" ref="AD2:AD27" si="5">INT(MAX(12 *(0.96*P2+Q2), MIN(12 *(0.96*P2+Q2+O2),  1900)  ))</f>
+        <f t="shared" ref="AD2:AD7" si="4">(12*E2+(12*D2 - 1000)*(D2&gt;450))</f>
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <f t="shared" ref="AF2:AF27" si="5">INT(MAX(12 *(0.96*R2+S2), MIN(12 *(0.96*R2+S2+Q2),  1900)  ))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A13" si="6">B3</f>
         <v>2</v>
@@ -718,85 +737,92 @@
         <v>2043</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <f>(N3=FALSE)*40+(N3=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J3" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K3" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>0</v>
       </c>
       <c r="L3" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
+      <c r="M3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
         <f>0.1*$D3</f>
         <v>60</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <f>0.02*D3</f>
         <v>12</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <f>0.08*D3</f>
         <v>48</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <f>0.015*D3</f>
         <v>9</v>
       </c>
-      <c r="R3" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>40</v>
-      </c>
-      <c r="T3">
+      <c r="T3" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="U3">
+        <v>40</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
         <v>2018</v>
       </c>
-      <c r="V3" s="2">
+      <c r="X3" s="2">
         <f t="shared" si="1"/>
         <v>4842</v>
       </c>
-      <c r="W3" s="2">
+      <c r="Y3" s="2">
         <f t="shared" si="2"/>
         <v>4842</v>
       </c>
-      <c r="X3" s="1">
-        <f>V3+MAX(F3*12-801,0)</f>
+      <c r="Z3" s="1">
+        <f>X3+MAX(F3*12-801,0)</f>
         <v>5241</v>
       </c>
-      <c r="Y3" s="1">
-        <f t="shared" ref="Y3:Y14" si="7">MAX(X3-AC3,0)</f>
+      <c r="AA3" s="1">
+        <f t="shared" ref="AA3:AA14" si="7">MAX(Z3-AE3,0)</f>
         <v>5241</v>
       </c>
-      <c r="AA3">
+      <c r="AC3">
         <f t="shared" si="3"/>
         <v>1322</v>
       </c>
-      <c r="AB3">
+      <c r="AD3">
         <f t="shared" si="4"/>
         <v>6200</v>
       </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
         <f t="shared" si="5"/>
         <v>804</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="6"/>
         <v>3</v>
@@ -824,85 +850,92 @@
         <v>2043</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <f>(N4=FALSE)*40+(N4=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K4" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K4">
         <v>0</v>
       </c>
       <c r="L4" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <f t="shared" ref="N4:N13" si="8">0.1*D4</f>
+      <c r="M4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P13" si="8">0.1*D4</f>
         <v>90</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <f>0.02*D4</f>
         <v>18</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <f>0.08*D4</f>
         <v>72</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <f>0.015*D4</f>
         <v>13.5</v>
       </c>
-      <c r="R4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>40</v>
-      </c>
-      <c r="T4">
+      <c r="T4" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="U4">
+        <v>40</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
         <v>2018</v>
       </c>
-      <c r="V4" s="2">
+      <c r="X4" s="2">
         <f t="shared" si="1"/>
         <v>7780</v>
       </c>
-      <c r="W4" s="2">
+      <c r="Y4" s="2">
         <f t="shared" si="2"/>
         <v>7780</v>
       </c>
-      <c r="X4" s="1">
-        <f>V4+MAX(F4*12-801,0)</f>
+      <c r="Z4" s="1">
+        <f>X4+MAX(F4*12-801,0)</f>
         <v>8179</v>
       </c>
-      <c r="Y4" s="1">
+      <c r="AA4" s="1">
         <f t="shared" si="7"/>
         <v>8179</v>
       </c>
-      <c r="AA4">
+      <c r="AC4">
         <f t="shared" si="3"/>
         <v>1984</v>
       </c>
-      <c r="AB4">
+      <c r="AD4">
         <f t="shared" si="4"/>
         <v>9800</v>
       </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
         <f t="shared" si="5"/>
         <v>1207</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="6"/>
         <v>4</v>
@@ -930,85 +963,92 @@
         <v>2043</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <f>(N5=FALSE)*40+(N5=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J5" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K5" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K5">
         <v>0</v>
       </c>
       <c r="L5" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
+      <c r="M5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
         <f t="shared" si="8"/>
         <v>120</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <f>0.02*D5</f>
         <v>24</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <f>0.08*D5</f>
         <v>96</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <f>0.015*D5</f>
         <v>18</v>
       </c>
-      <c r="R5" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>40</v>
-      </c>
-      <c r="T5">
+      <c r="T5" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="U5">
+        <v>40</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
         <v>2018</v>
       </c>
-      <c r="V5" s="2">
+      <c r="X5" s="2">
         <f t="shared" si="1"/>
         <v>10719</v>
       </c>
-      <c r="W5" s="2">
+      <c r="Y5" s="2">
         <f t="shared" si="2"/>
         <v>10719</v>
       </c>
-      <c r="X5" s="1">
-        <f>V5+MAX(F5*12-801,0)</f>
+      <c r="Z5" s="1">
+        <f>X5+MAX(F5*12-801,0)</f>
         <v>11118</v>
       </c>
-      <c r="Y5" s="1">
+      <c r="AA5" s="1">
         <f t="shared" si="7"/>
         <v>11118</v>
       </c>
-      <c r="AA5">
+      <c r="AC5">
         <f t="shared" si="3"/>
         <v>2645</v>
       </c>
-      <c r="AB5">
+      <c r="AD5">
         <f t="shared" si="4"/>
         <v>13400</v>
       </c>
-      <c r="AC5">
-        <v>0</v>
-      </c>
-      <c r="AD5">
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
         <f t="shared" si="5"/>
         <v>1609</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="6"/>
         <v>5</v>
@@ -1036,85 +1076,92 @@
         <v>2043</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <f>(N6=FALSE)*40+(N6=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K6" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K6">
         <v>0</v>
       </c>
       <c r="L6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
+      <c r="M6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="8"/>
         <v>150</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <f>0.02*D6</f>
         <v>30</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <f>0.08*D6</f>
         <v>120</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <f>0.015*D6</f>
         <v>22.5</v>
       </c>
-      <c r="R6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>40</v>
-      </c>
-      <c r="T6">
+      <c r="T6" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="U6">
+        <v>40</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
         <v>2018</v>
       </c>
-      <c r="V6" s="2">
+      <c r="X6" s="2">
         <f t="shared" si="1"/>
         <v>13768</v>
       </c>
-      <c r="W6" s="2">
+      <c r="Y6" s="2">
         <f t="shared" si="2"/>
         <v>13768</v>
       </c>
-      <c r="X6" s="1">
-        <f>V6+MAX(F6*12-801,0)</f>
+      <c r="Z6" s="1">
+        <f>X6+MAX(F6*12-801,0)</f>
         <v>14167</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="AA6" s="1">
         <f t="shared" si="7"/>
         <v>14167</v>
       </c>
-      <c r="AA6">
+      <c r="AC6">
         <f t="shared" si="3"/>
         <v>3196</v>
       </c>
-      <c r="AB6">
+      <c r="AD6">
         <f t="shared" si="4"/>
         <v>17000</v>
       </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
-      <c r="AD6">
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
         <f t="shared" si="5"/>
         <v>1900</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="6"/>
         <v>6</v>
@@ -1142,85 +1189,92 @@
         <v>2043</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <f>(N7=FALSE)*40+(N7=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K7" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K7">
         <v>0</v>
       </c>
       <c r="L7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
+      <c r="M7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="8"/>
         <v>500</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <f>0.02*D7</f>
         <v>100</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <f>0.08*D7</f>
         <v>400</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <f>0.015*D7</f>
         <v>75</v>
       </c>
-      <c r="R7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>40</v>
-      </c>
-      <c r="T7">
+      <c r="T7" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="U7">
+        <v>40</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
         <v>2018</v>
       </c>
-      <c r="V7" s="2">
+      <c r="X7" s="2">
         <f t="shared" si="1"/>
         <v>49136</v>
       </c>
-      <c r="W7" s="2">
+      <c r="Y7" s="2">
         <f t="shared" si="2"/>
         <v>49136</v>
       </c>
-      <c r="X7" s="1">
-        <f>V7+MAX(F7*12-801,0)</f>
+      <c r="Z7" s="1">
+        <f>X7+MAX(F7*12-801,0)</f>
         <v>49535</v>
       </c>
-      <c r="Y7" s="1">
+      <c r="AA7" s="1">
         <f t="shared" si="7"/>
         <v>49535</v>
       </c>
-      <c r="AA7">
+      <c r="AC7">
         <f t="shared" si="3"/>
         <v>9828</v>
       </c>
-      <c r="AB7">
+      <c r="AD7">
         <f t="shared" si="4"/>
         <v>59000</v>
       </c>
-      <c r="AC7">
-        <v>0</v>
-      </c>
-      <c r="AD7">
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
         <f t="shared" si="5"/>
         <v>5508</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="6"/>
         <v>7</v>
@@ -1248,24 +1302,25 @@
         <v>2035</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <f>(N8=FALSE)*40+(N8=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J8" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K8" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K8">
         <v>0</v>
       </c>
       <c r="L8" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
+      <c r="M8" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N8" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="O8">
@@ -1277,52 +1332,58 @@
       <c r="Q8">
         <v>0</v>
       </c>
-      <c r="R8" t="b">
-        <f>FALSE</f>
+      <c r="R8">
         <v>0</v>
       </c>
       <c r="S8">
-        <v>40</v>
-      </c>
-      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="T8" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="U8">
+        <v>40</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
         <v>2010</v>
       </c>
-      <c r="V8" s="2">
+      <c r="X8" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W8" s="2">
+      <c r="Y8" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X8" s="1">
-        <f>V8+MAX(F8*12-801-36,0)</f>
+      <c r="Z8" s="1">
+        <f>X8+MAX(F8*12-801-36,0)</f>
         <v>363</v>
       </c>
-      <c r="Y8" s="1">
+      <c r="AA8" s="1">
         <f t="shared" si="7"/>
         <v>363</v>
       </c>
-      <c r="AA8">
+      <c r="AC8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AB8">
-        <f t="shared" ref="AB8:AB13" si="9">(12*E8+(12*D8 - 920)*(D8&gt;450))</f>
-        <v>0</v>
-      </c>
-      <c r="AC8">
-        <v>0</v>
-      </c>
       <c r="AD8">
+        <f t="shared" ref="AD8:AD13" si="9">(12*E8+(12*D8 - 920)*(D8&gt;450))</f>
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="6"/>
         <v>8</v>
@@ -1350,85 +1411,92 @@
         <v>2035</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <f>(N9=FALSE)*40+(N9=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K9" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K9">
         <v>0</v>
       </c>
       <c r="L9" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
+      <c r="M9" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N9" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="8"/>
         <v>60</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <f>0.02*D9</f>
         <v>12</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <f>0.08*D9</f>
         <v>48</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <f>0.015*D9</f>
         <v>9</v>
       </c>
-      <c r="R9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>40</v>
-      </c>
-      <c r="T9">
+      <c r="T9" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="U9">
+        <v>40</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
         <v>2010</v>
       </c>
-      <c r="V9" s="2">
+      <c r="X9" s="2">
         <f t="shared" si="1"/>
         <v>5152</v>
       </c>
-      <c r="W9" s="2">
+      <c r="Y9" s="2">
         <f t="shared" si="2"/>
         <v>5152</v>
       </c>
-      <c r="X9" s="1">
-        <f t="shared" ref="X9:X14" si="10">V9+MAX(F9*12-801,0)</f>
+      <c r="Z9" s="1">
+        <f t="shared" ref="Z9:Z14" si="10">X9+MAX(F9*12-801,0)</f>
         <v>5551</v>
       </c>
-      <c r="Y9" s="1">
+      <c r="AA9" s="1">
         <f t="shared" si="7"/>
         <v>5551</v>
       </c>
-      <c r="AA9">
+      <c r="AC9">
         <f t="shared" si="3"/>
         <v>1092</v>
       </c>
-      <c r="AB9">
+      <c r="AD9">
         <f t="shared" si="9"/>
         <v>6280</v>
       </c>
-      <c r="AC9">
-        <v>0</v>
-      </c>
-      <c r="AD9">
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
         <f t="shared" si="5"/>
         <v>804</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="6"/>
         <v>9</v>
@@ -1456,85 +1524,92 @@
         <v>2035</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <f>(N10=FALSE)*40+(N10=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K10" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K10">
         <v>0</v>
       </c>
       <c r="L10" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
+      <c r="M10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="8"/>
         <v>90</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <f>0.02*D10</f>
         <v>18</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <f>0.08*D10</f>
         <v>72</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <f>0.015*D10</f>
         <v>13.5</v>
       </c>
-      <c r="R10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>40</v>
-      </c>
-      <c r="T10">
+      <c r="T10" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="U10">
+        <v>40</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
         <v>2010</v>
       </c>
-      <c r="V10" s="2">
+      <c r="X10" s="2">
         <f t="shared" si="1"/>
         <v>8205</v>
       </c>
-      <c r="W10" s="2">
+      <c r="Y10" s="2">
         <f t="shared" si="2"/>
         <v>8205</v>
       </c>
-      <c r="X10" s="1">
+      <c r="Z10" s="1">
         <f t="shared" si="10"/>
         <v>8604</v>
       </c>
-      <c r="Y10" s="1">
+      <c r="AA10" s="1">
         <f t="shared" si="7"/>
         <v>8604</v>
       </c>
-      <c r="AA10">
+      <c r="AC10">
         <f t="shared" si="3"/>
         <v>1639</v>
       </c>
-      <c r="AB10">
+      <c r="AD10">
         <f t="shared" si="9"/>
         <v>9880</v>
       </c>
-      <c r="AC10">
-        <v>0</v>
-      </c>
-      <c r="AD10">
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
         <f t="shared" si="5"/>
         <v>1207</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="6"/>
         <v>10</v>
@@ -1562,85 +1637,92 @@
         <v>2035</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <f>(N11=FALSE)*40+(N11=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J11" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K11" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K11">
         <v>0</v>
       </c>
       <c r="L11" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
+      <c r="M11" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N11" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="8"/>
         <v>120</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <f>0.02*D11</f>
         <v>24</v>
       </c>
-      <c r="P11">
+      <c r="R11">
         <f>0.08*D11</f>
         <v>96</v>
       </c>
-      <c r="Q11">
+      <c r="S11">
         <f>0.015*D11</f>
         <v>18</v>
       </c>
-      <c r="R11" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>40</v>
-      </c>
-      <c r="T11">
+      <c r="T11" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="U11">
+        <v>40</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
         <v>2010</v>
       </c>
-      <c r="V11" s="2">
+      <c r="X11" s="2">
         <f t="shared" si="1"/>
         <v>11259</v>
       </c>
-      <c r="W11" s="2">
+      <c r="Y11" s="2">
         <f t="shared" si="2"/>
         <v>11259</v>
       </c>
-      <c r="X11" s="1">
+      <c r="Z11" s="1">
         <f t="shared" si="10"/>
         <v>11658</v>
       </c>
-      <c r="Y11" s="1">
+      <c r="AA11" s="1">
         <f t="shared" si="7"/>
         <v>11658</v>
       </c>
-      <c r="AA11">
+      <c r="AC11">
         <f t="shared" si="3"/>
         <v>2185</v>
       </c>
-      <c r="AB11">
+      <c r="AD11">
         <f t="shared" si="9"/>
         <v>13480</v>
       </c>
-      <c r="AC11">
-        <v>0</v>
-      </c>
-      <c r="AD11">
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
         <f t="shared" si="5"/>
         <v>1609</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="6"/>
         <v>11</v>
@@ -1668,85 +1750,92 @@
         <v>2035</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <f>(N12=FALSE)*40+(N12=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J12" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K12" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K12">
         <v>0</v>
       </c>
       <c r="L12" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
+      <c r="M12" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N12" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
         <f t="shared" si="8"/>
         <v>150</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <f>0.02*D12</f>
         <v>30</v>
       </c>
-      <c r="P12">
+      <c r="R12">
         <f>0.08*D12</f>
         <v>120</v>
       </c>
-      <c r="Q12">
+      <c r="S12">
         <f>0.015*D12</f>
         <v>22.5</v>
       </c>
-      <c r="R12" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>40</v>
-      </c>
-      <c r="T12">
+      <c r="T12" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="U12">
+        <v>40</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
         <v>2010</v>
       </c>
-      <c r="V12" s="2">
+      <c r="X12" s="2">
         <f t="shared" si="1"/>
         <v>14424</v>
       </c>
-      <c r="W12" s="2">
+      <c r="Y12" s="2">
         <f t="shared" si="2"/>
         <v>14424</v>
       </c>
-      <c r="X12" s="1">
+      <c r="Z12" s="1">
         <f t="shared" si="10"/>
         <v>14823</v>
       </c>
-      <c r="Y12" s="1">
+      <c r="AA12" s="1">
         <f t="shared" si="7"/>
         <v>14823</v>
       </c>
-      <c r="AA12">
+      <c r="AC12">
         <f t="shared" si="3"/>
         <v>2620</v>
       </c>
-      <c r="AB12">
+      <c r="AD12">
         <f t="shared" si="9"/>
         <v>17080</v>
       </c>
-      <c r="AC12">
-        <v>0</v>
-      </c>
-      <c r="AD12">
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
         <f t="shared" si="5"/>
         <v>1900</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="6"/>
         <v>12</v>
@@ -1774,85 +1863,92 @@
         <v>2035</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <f>(N13=FALSE)*40+(N13=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J13" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K13" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K13">
         <v>0</v>
       </c>
       <c r="L13" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
+      <c r="M13" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N13" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
         <f t="shared" si="8"/>
         <v>800</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <f>0.02*D13</f>
         <v>160</v>
       </c>
-      <c r="P13">
+      <c r="R13">
         <f>0.08*D13</f>
         <v>640</v>
       </c>
-      <c r="Q13">
+      <c r="S13">
         <f>0.015*D13</f>
         <v>120</v>
       </c>
-      <c r="R13" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S13">
-        <v>40</v>
-      </c>
-      <c r="T13">
+      <c r="T13" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="U13">
+        <v>40</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
         <v>2010</v>
       </c>
-      <c r="V13" s="2">
+      <c r="X13" s="2">
         <f t="shared" si="1"/>
         <v>83606</v>
       </c>
-      <c r="W13" s="2">
+      <c r="Y13" s="2">
         <f t="shared" si="2"/>
         <v>83606</v>
       </c>
-      <c r="X13" s="1">
+      <c r="Z13" s="1">
         <f t="shared" si="10"/>
         <v>84005</v>
       </c>
-      <c r="Y13" s="1">
+      <c r="AA13" s="1">
         <f t="shared" si="7"/>
         <v>84005</v>
       </c>
-      <c r="AA13">
-        <f>INT(((0.6+(0.02*(U13-2005)))*(12*2*0.0995*5500))-(12*0.0995*5500))+AD13</f>
+      <c r="AC13">
+        <f>INT(((0.6+(0.02*(W13-2005)))*(12*2*0.0995*5500))-(12*0.0995*5500))+AF13</f>
         <v>11438</v>
       </c>
-      <c r="AB13">
+      <c r="AD13">
         <f t="shared" si="9"/>
         <v>95080</v>
       </c>
-      <c r="AC13">
-        <v>0</v>
-      </c>
-      <c r="AD13">
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
         <f t="shared" si="5"/>
         <v>8812</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>21</v>
       </c>
@@ -1879,86 +1975,93 @@
         <v>2037</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <f>(N14=FALSE)*40+(N14=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J14" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K14" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K14">
         <v>0</v>
       </c>
       <c r="L14" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
+      <c r="M14" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N14" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
         <f>0.1*$D14</f>
         <v>200</v>
       </c>
-      <c r="O14">
-        <f t="shared" ref="O14:O19" si="11">0.02*D14</f>
-        <v>40</v>
-      </c>
-      <c r="P14">
-        <f t="shared" ref="P14:P19" si="12">0.08*D14</f>
+      <c r="Q14">
+        <f t="shared" ref="Q14:Q19" si="11">0.02*D14</f>
+        <v>40</v>
+      </c>
+      <c r="R14">
+        <f t="shared" ref="R14:R19" si="12">0.08*D14</f>
         <v>160</v>
       </c>
-      <c r="Q14">
-        <f t="shared" ref="Q14:Q19" si="13">0.015*D14</f>
+      <c r="S14">
+        <f t="shared" ref="S14:S19" si="13">0.015*D14</f>
         <v>30</v>
       </c>
-      <c r="R14" t="b">
+      <c r="T14" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="S14">
-        <v>40</v>
-      </c>
-      <c r="T14">
-        <v>1</v>
-      </c>
       <c r="U14">
+        <v>40</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
         <v>2012</v>
       </c>
-      <c r="V14" s="2">
-        <f>MAX(AB14-AA14-36-1308,0)</f>
+      <c r="X14" s="2">
+        <f>MAX(AD14-AC14-36-1308,0)</f>
         <v>18301</v>
       </c>
-      <c r="W14" s="2">
+      <c r="Y14" s="2">
         <f t="shared" si="2"/>
         <v>14797</v>
       </c>
-      <c r="X14" s="1">
+      <c r="Z14" s="1">
         <f t="shared" si="10"/>
         <v>18700</v>
       </c>
-      <c r="Y14" s="1">
+      <c r="AA14" s="1">
         <f t="shared" si="7"/>
         <v>15196</v>
       </c>
-      <c r="AA14">
-        <f t="shared" ref="AA14:AA27" si="14">INT(((0.6+(0.02*(U14-2005)))*(2*12*N14))-(12*N14))+AD14</f>
+      <c r="AC14">
+        <f t="shared" ref="AC14:AC27" si="14">INT(((0.6+(0.02*(W14-2005)))*(2*12*P14))-(12*P14))+AF14</f>
         <v>3355</v>
       </c>
-      <c r="AB14">
+      <c r="AD14">
         <f>(12*E14+(12*D14 - 1000)*(D14&gt;450))</f>
         <v>23000</v>
       </c>
-      <c r="AC14">
+      <c r="AE14">
         <f>0.5*7008</f>
         <v>3504</v>
       </c>
-      <c r="AD14">
+      <c r="AF14">
         <f t="shared" si="5"/>
         <v>2203</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>21</v>
       </c>
@@ -1985,73 +2088,80 @@
         <v>2072</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <f>(N15=FALSE)*40+(N15=TRUE)</f>
+        <v>1</v>
       </c>
       <c r="J15" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K15" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K15">
         <v>0</v>
       </c>
       <c r="L15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="M15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N15" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
         <f>0.1*$D15</f>
         <v>0</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P15">
+      <c r="R15">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="Q15">
+      <c r="S15">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="R15" t="b">
+      <c r="T15" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="S15">
+      <c r="U15">
         <v>5</v>
       </c>
-      <c r="T15">
-        <v>1</v>
-      </c>
-      <c r="U15">
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15">
         <v>2012</v>
       </c>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="AA15">
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AC15">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AB15">
+      <c r="AD15">
         <f>(12*E15+(12*D15 - 1000)*(D15&gt;450))</f>
         <v>0</v>
       </c>
-      <c r="AC15">
-        <v>0</v>
-      </c>
-      <c r="AD15">
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>22</v>
       </c>
@@ -2078,86 +2188,93 @@
         <v>2034</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <f>(N16=FALSE)*40+(N16=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J16" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K16" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K16">
         <v>0</v>
       </c>
       <c r="L16" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <f t="shared" ref="N16:N19" si="15">0.1*D16</f>
+      <c r="M16" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N16" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <f t="shared" ref="P16:P19" si="15">0.1*D16</f>
         <v>300</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <f t="shared" si="11"/>
         <v>60</v>
       </c>
-      <c r="P16">
+      <c r="R16">
         <f t="shared" si="12"/>
         <v>240</v>
       </c>
-      <c r="Q16">
+      <c r="S16">
         <f t="shared" si="13"/>
         <v>45</v>
       </c>
-      <c r="R16" t="b">
+      <c r="T16" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="S16">
-        <v>40</v>
-      </c>
-      <c r="T16">
-        <v>1</v>
-      </c>
       <c r="U16">
+        <v>40</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16">
         <v>2009</v>
       </c>
-      <c r="V16" s="2">
-        <f>MAX(AB16-AA16-36-1308,0)</f>
+      <c r="X16" s="2">
+        <f>MAX(AD16-AC16-36-1308,0)</f>
         <v>29136</v>
       </c>
-      <c r="W16" s="2">
-        <f>V16-AC16</f>
+      <c r="Y16" s="2">
+        <f>X16-AE16</f>
         <v>26124</v>
       </c>
-      <c r="X16" s="1">
-        <f>V16+MAX(F16*12-801,0)</f>
+      <c r="Z16" s="1">
+        <f>X16+MAX(F16*12-801,0)</f>
         <v>29535</v>
       </c>
-      <c r="Y16" s="1">
-        <f>MAX(X16-AC16,0)</f>
+      <c r="AA16" s="1">
+        <f>MAX(Z16-AE16,0)</f>
         <v>26523</v>
       </c>
-      <c r="AA16">
+      <c r="AC16">
         <f t="shared" si="14"/>
         <v>4600</v>
       </c>
-      <c r="AB16">
+      <c r="AD16">
         <f>(12*E16+(12*D16 - 920)*(D16&gt;450))</f>
         <v>35080</v>
       </c>
-      <c r="AC16">
+      <c r="AE16">
         <f>0.5*6024</f>
         <v>3012</v>
       </c>
-      <c r="AD16">
+      <c r="AF16">
         <f t="shared" si="5"/>
         <v>3304</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>22</v>
       </c>
@@ -2184,73 +2301,80 @@
         <v>2069</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <f>(N17=FALSE)*40+(N17=TRUE)</f>
+        <v>1</v>
       </c>
       <c r="J17" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K17" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K17">
         <v>0</v>
       </c>
       <c r="L17" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="M17" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N17" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P17">
+      <c r="R17">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="Q17">
+      <c r="S17">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="R17" t="b">
+      <c r="T17" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="S17">
+      <c r="U17">
         <v>5</v>
       </c>
-      <c r="T17">
-        <v>1</v>
-      </c>
-      <c r="U17">
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17">
         <v>2009</v>
       </c>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="AA17">
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AC17">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AB17">
+      <c r="AD17">
         <f>(12*E17+(12*D17 - 1000)*(D17&gt;450))</f>
         <v>0</v>
       </c>
-      <c r="AC17">
-        <v>0</v>
-      </c>
-      <c r="AD17">
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>23</v>
       </c>
@@ -2277,86 +2401,93 @@
         <v>2030</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <f>(N18=FALSE)*40+(N18=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J18" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K18" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K18">
         <v>0</v>
       </c>
       <c r="L18" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
+      <c r="M18" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N18" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
         <f t="shared" si="15"/>
         <v>200</v>
       </c>
-      <c r="O18">
+      <c r="Q18">
         <f t="shared" si="11"/>
         <v>40</v>
       </c>
-      <c r="P18">
+      <c r="R18">
         <f t="shared" si="12"/>
         <v>160</v>
       </c>
-      <c r="Q18">
+      <c r="S18">
         <f t="shared" si="13"/>
         <v>30</v>
       </c>
-      <c r="R18" t="b">
+      <c r="T18" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="S18">
-        <v>40</v>
-      </c>
-      <c r="T18">
-        <v>1</v>
-      </c>
       <c r="U18">
+        <v>40</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18">
         <v>2005</v>
       </c>
-      <c r="V18" s="2">
-        <f>MAX(AB18-AA18-36-1308,0)</f>
+      <c r="X18" s="2">
+        <f>MAX(AD18-AC18-36-1308,0)</f>
         <v>29632</v>
       </c>
-      <c r="W18" s="2">
-        <f>V18-AC18</f>
+      <c r="Y18" s="2">
+        <f>X18-AE18</f>
         <v>26728</v>
       </c>
-      <c r="X18" s="1">
-        <f>V18+MAX(F18*12-1370-51,0)</f>
+      <c r="Z18" s="1">
+        <f>X18+MAX(F18*12-1370-51,0)</f>
         <v>40211</v>
       </c>
-      <c r="Y18" s="1">
-        <f>MAX(X18-AC18,0)</f>
+      <c r="AA18" s="1">
+        <f>MAX(Z18-AE18,0)</f>
         <v>37307</v>
       </c>
-      <c r="AA18">
+      <c r="AC18">
         <f t="shared" si="14"/>
         <v>2683</v>
       </c>
-      <c r="AB18">
+      <c r="AD18">
         <f>(12*E18+((12*D18)-920)*(D18&gt;450)+MAX((12*F18)-51-1370,0))</f>
         <v>33659</v>
       </c>
-      <c r="AC18">
+      <c r="AE18">
         <f>5808/2</f>
         <v>2904</v>
       </c>
-      <c r="AD18">
+      <c r="AF18">
         <f t="shared" si="5"/>
         <v>2203</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>23</v>
       </c>
@@ -2383,73 +2514,80 @@
         <v>2065</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <f>(N19=FALSE)*40+(N19=TRUE)</f>
+        <v>1</v>
       </c>
       <c r="J19" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K19" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K19">
         <v>0</v>
       </c>
       <c r="L19" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="M19" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N19" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="O19">
+      <c r="Q19">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P19">
+      <c r="R19">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="Q19">
+      <c r="S19">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="R19" t="b">
+      <c r="T19" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="S19">
+      <c r="U19">
         <v>5</v>
       </c>
-      <c r="T19">
-        <v>1</v>
-      </c>
-      <c r="U19">
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19">
         <v>2005</v>
       </c>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="AA19">
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AC19">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AB19">
-        <f t="shared" ref="AB19:AB30" si="16">(12*E19+(12*D19 - 1000)*(D19&gt;450))</f>
-        <v>0</v>
-      </c>
-      <c r="AC19">
-        <v>0</v>
-      </c>
       <c r="AD19">
+        <f t="shared" ref="AD19:AD30" si="16">(12*E19+(12*D19 - 1000)*(D19&gt;450))</f>
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>31</v>
       </c>
@@ -2472,89 +2610,96 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <f>U20+(65-S20)</f>
+        <f>W20+(65-U20)</f>
         <v>2053</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <f>(N20=FALSE)*40+(N20=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J20" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K20" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K20">
         <v>0</v>
       </c>
       <c r="L20" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
+      <c r="M20" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N20" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
         <f>0.1*$D20</f>
         <v>200</v>
       </c>
-      <c r="O20">
+      <c r="Q20">
         <f>0.02*D20</f>
         <v>40</v>
       </c>
-      <c r="P20">
+      <c r="R20">
         <f>0.08*D20</f>
         <v>160</v>
       </c>
-      <c r="Q20">
+      <c r="S20">
         <f>0.015*D20</f>
         <v>30</v>
       </c>
-      <c r="R20" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S20">
+      <c r="T20" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="U20">
         <v>30</v>
       </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
-      <c r="U20">
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
         <v>2018</v>
       </c>
-      <c r="V20" s="2">
-        <f>MAX(AB20-AA20-36,0)</f>
+      <c r="X20" s="2">
+        <f>MAX(AD20-AC20-36,0)</f>
         <v>19033</v>
       </c>
-      <c r="W20" s="2">
-        <f>V20-AC20</f>
+      <c r="Y20" s="2">
+        <f>X20-AE20</f>
         <v>19033</v>
       </c>
-      <c r="X20" s="1">
-        <f>V20+MAX(F20*12-801,0)</f>
+      <c r="Z20" s="1">
+        <f>X20+MAX(F20*12-801,0)</f>
         <v>19033</v>
       </c>
-      <c r="Y20" s="1">
-        <f>MAX(X20-AC20,0)</f>
+      <c r="AA20" s="1">
+        <f>MAX(Z20-AE20,0)</f>
         <v>19033</v>
       </c>
-      <c r="AA20">
+      <c r="AC20">
         <f t="shared" si="14"/>
         <v>3931</v>
       </c>
-      <c r="AB20">
+      <c r="AD20">
         <f t="shared" si="16"/>
         <v>23000</v>
       </c>
-      <c r="AC20">
-        <v>0</v>
-      </c>
-      <c r="AD20">
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
         <f t="shared" si="5"/>
         <v>2203</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>31</v>
       </c>
@@ -2577,89 +2722,96 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <f t="shared" ref="H21:H27" si="17">U21+(65-S21)</f>
+        <f t="shared" ref="H21:H27" si="17">W21+(65-U21)</f>
         <v>2053</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <f>(N21=FALSE)*40+(N21=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J21" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K21" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K21">
         <v>0</v>
       </c>
       <c r="L21" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <f t="shared" ref="N21:N30" si="18">0.1*$D21</f>
+      <c r="M21" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N21" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <f t="shared" ref="P21:P30" si="18">0.1*$D21</f>
         <v>100</v>
       </c>
-      <c r="O21">
-        <f t="shared" ref="O21:O25" si="19">0.02*D21</f>
+      <c r="Q21">
+        <f t="shared" ref="Q21:Q25" si="19">0.02*D21</f>
         <v>20</v>
       </c>
-      <c r="P21">
-        <f t="shared" ref="P21:P25" si="20">0.08*D21</f>
+      <c r="R21">
+        <f t="shared" ref="R21:R25" si="20">0.08*D21</f>
         <v>80</v>
       </c>
-      <c r="Q21">
-        <f t="shared" ref="Q21:Q25" si="21">0.015*D21</f>
+      <c r="S21">
+        <f t="shared" ref="S21:S25" si="21">0.015*D21</f>
         <v>15</v>
       </c>
-      <c r="R21" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S21">
+      <c r="T21" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="U21">
         <v>30</v>
       </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
         <v>2018</v>
       </c>
-      <c r="V21" s="2">
-        <f>MAX(AB21-AA21-36,0)</f>
+      <c r="X21" s="2">
+        <f>MAX(AD21-AC21-36,0)</f>
         <v>8759</v>
       </c>
-      <c r="W21" s="2">
-        <f>V21-AC21</f>
+      <c r="Y21" s="2">
+        <f>X21-AE21</f>
         <v>8759</v>
       </c>
-      <c r="X21" s="1">
-        <f>V21+MAX(F21*12-801,0)</f>
+      <c r="Z21" s="1">
+        <f>X21+MAX(F21*12-801,0)</f>
         <v>8759</v>
       </c>
-      <c r="Y21" s="1">
-        <f>MAX(X21-AC21,0)</f>
+      <c r="AA21" s="1">
+        <f>MAX(Z21-AE21,0)</f>
         <v>8759</v>
       </c>
-      <c r="AA21">
+      <c r="AC21">
         <f t="shared" si="14"/>
         <v>2205</v>
       </c>
-      <c r="AB21">
+      <c r="AD21">
         <f t="shared" si="16"/>
         <v>11000</v>
       </c>
-      <c r="AC21">
-        <v>0</v>
-      </c>
-      <c r="AD21">
+      <c r="AE21">
+        <v>0</v>
+      </c>
+      <c r="AF21">
         <f t="shared" si="5"/>
         <v>1341</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>32</v>
       </c>
@@ -2686,86 +2838,93 @@
         <v>2053</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <f>(N22=FALSE)*40+(N22=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J22" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="M22" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="L22" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
+      <c r="N22" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
         <f t="shared" si="18"/>
         <v>300</v>
       </c>
-      <c r="O22">
+      <c r="Q22">
         <f t="shared" si="19"/>
         <v>60</v>
       </c>
-      <c r="P22">
+      <c r="R22">
         <f t="shared" si="20"/>
         <v>240</v>
       </c>
-      <c r="Q22">
+      <c r="S22">
         <f t="shared" si="21"/>
         <v>45</v>
       </c>
-      <c r="R22" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S22">
+      <c r="T22" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="U22">
         <v>30</v>
       </c>
-      <c r="T22">
+      <c r="V22">
         <v>2</v>
       </c>
-      <c r="U22">
+      <c r="W22">
         <v>2018</v>
       </c>
-      <c r="V22" s="2">
-        <f>0.5*(AB22+AB23-(AA22+AA23)-2*36)</f>
+      <c r="X22" s="2">
+        <f>0.5*(AD22+AD23-(AC22+AC23)-2*36)</f>
         <v>24050.5</v>
       </c>
-      <c r="W22" s="2">
-        <f>V22-AC22</f>
+      <c r="Y22" s="2">
+        <f>X22-AE22</f>
         <v>16622.5</v>
       </c>
-      <c r="X22" s="1">
-        <f>V22+MAX(0.5*(F22*12-(2*801)),0)</f>
+      <c r="Z22" s="1">
+        <f>X22+MAX(0.5*(F22*12-(2*801)),0)</f>
         <v>24449.5</v>
       </c>
-      <c r="Y22" s="1">
-        <f>MAX(X22-AC22,0)</f>
+      <c r="AA22" s="1">
+        <f>MAX(Z22-AE22,0)</f>
         <v>17021.5</v>
       </c>
-      <c r="AA22">
+      <c r="AC22">
         <f t="shared" si="14"/>
         <v>5896</v>
       </c>
-      <c r="AB22">
+      <c r="AD22">
         <f t="shared" si="16"/>
         <v>35000</v>
       </c>
-      <c r="AC22">
+      <c r="AE22">
         <f>7428/2*2</f>
         <v>7428</v>
       </c>
-      <c r="AD22">
+      <c r="AF22">
         <f t="shared" si="5"/>
         <v>3304</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>32</v>
       </c>
@@ -2792,86 +2951,93 @@
         <v>2053</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <f>(N23=FALSE)*40+(N23=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J23" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="M23" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="L23" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23">
+      <c r="N23" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
         <f t="shared" si="18"/>
         <v>200</v>
       </c>
-      <c r="O23">
+      <c r="Q23">
         <f t="shared" si="19"/>
         <v>40</v>
       </c>
-      <c r="P23">
+      <c r="R23">
         <f t="shared" si="20"/>
         <v>160</v>
       </c>
-      <c r="Q23">
+      <c r="S23">
         <f t="shared" si="21"/>
         <v>30</v>
       </c>
-      <c r="R23" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S23">
+      <c r="T23" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="U23">
         <v>30</v>
       </c>
-      <c r="T23">
+      <c r="V23">
         <v>2</v>
       </c>
-      <c r="U23">
+      <c r="W23">
         <v>2018</v>
       </c>
-      <c r="V23" s="2">
-        <f>0.5*(AB22+AB23-(AA22+AA23)-2*36)</f>
+      <c r="X23" s="2">
+        <f>0.5*(AD22+AD23-(AC22+AC23)-2*36)</f>
         <v>24050.5</v>
       </c>
-      <c r="W23" s="2">
-        <f>V23-AC23</f>
+      <c r="Y23" s="2">
+        <f>X23-AE23</f>
         <v>16622.5</v>
       </c>
-      <c r="X23" s="1">
-        <f>V22+MAX(0.5*(F22*12-(2*801)),0)</f>
+      <c r="Z23" s="1">
+        <f>X22+MAX(0.5*(F22*12-(2*801)),0)</f>
         <v>24449.5</v>
       </c>
-      <c r="Y23" s="1">
-        <f>MAX(X23-AC23,0)</f>
+      <c r="AA23" s="1">
+        <f>MAX(Z23-AE23,0)</f>
         <v>17021.5</v>
       </c>
-      <c r="AA23">
+      <c r="AC23">
         <f t="shared" si="14"/>
         <v>3931</v>
       </c>
-      <c r="AB23">
+      <c r="AD23">
         <f t="shared" si="16"/>
         <v>23000</v>
       </c>
-      <c r="AC23">
+      <c r="AE23">
         <f>7428/2*2</f>
         <v>7428</v>
       </c>
-      <c r="AD23">
+      <c r="AF23">
         <f t="shared" si="5"/>
         <v>2203</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>32</v>
       </c>
@@ -2898,73 +3064,80 @@
         <v>2075</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <f>(N24=FALSE)*40+(N24=TRUE)</f>
+        <v>1</v>
       </c>
       <c r="J24" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K24" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K24">
         <v>0</v>
       </c>
       <c r="L24" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="M24" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N24" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24">
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="O24">
+      <c r="Q24">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P24">
+      <c r="R24">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="Q24">
+      <c r="S24">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="R24" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S24">
+      <c r="T24" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="U24">
         <v>8</v>
       </c>
-      <c r="T24">
+      <c r="V24">
         <v>2</v>
       </c>
-      <c r="U24">
+      <c r="W24">
         <v>2018</v>
       </c>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-      <c r="AA24">
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AC24">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AB24">
+      <c r="AD24">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AC24">
-        <v>0</v>
-      </c>
-      <c r="AD24">
+      <c r="AE24">
+        <v>0</v>
+      </c>
+      <c r="AF24">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>32</v>
       </c>
@@ -2991,73 +3164,80 @@
         <v>2080</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <f>(N25=FALSE)*40+(N25=TRUE)</f>
+        <v>1</v>
       </c>
       <c r="J25" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K25" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K25">
         <v>0</v>
       </c>
       <c r="L25" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="M25" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N25" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25">
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="O25">
+      <c r="Q25">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P25">
+      <c r="R25">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="Q25">
+      <c r="S25">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="R25" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S25">
+      <c r="T25" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="U25">
         <v>3</v>
       </c>
-      <c r="T25">
+      <c r="V25">
         <v>2</v>
       </c>
-      <c r="U25">
+      <c r="W25">
         <v>2018</v>
       </c>
-      <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="AA25">
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+      <c r="AC25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AB25">
+      <c r="AD25">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AC25">
-        <v>0</v>
-      </c>
-      <c r="AD25">
+      <c r="AE25">
+        <v>0</v>
+      </c>
+      <c r="AF25">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>33</v>
       </c>
@@ -3083,101 +3263,108 @@
         <f t="shared" si="17"/>
         <v>2043</v>
       </c>
-      <c r="I26" s="3">
-        <v>0</v>
-      </c>
-      <c r="J26" s="3" t="b">
+      <c r="I26">
+        <f>(N26=FALSE)*40+(N26=TRUE)</f>
+        <v>40</v>
+      </c>
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0</v>
+      </c>
+      <c r="L26" s="3" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="K26" s="3" t="b">
+      <c r="M26" s="3" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="L26" s="3" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="M26" s="3">
+      <c r="N26" s="3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O26" s="3">
         <v>50</v>
       </c>
-      <c r="N26" s="3">
+      <c r="P26" s="3">
         <f>0.093*5800</f>
         <v>539.4</v>
       </c>
-      <c r="O26" s="3">
-        <f t="shared" ref="O26:O30" si="22">0.02*D26</f>
+      <c r="Q26" s="3">
+        <f t="shared" ref="Q26:Q30" si="22">0.02*D26</f>
         <v>140</v>
       </c>
-      <c r="P26" s="3">
-        <f t="shared" ref="P26:P30" si="23">0.08*D26</f>
+      <c r="R26" s="3">
+        <f t="shared" ref="R26:R30" si="23">0.08*D26</f>
         <v>560</v>
       </c>
-      <c r="Q26" s="3">
-        <f t="shared" ref="Q26:Q30" si="24">0.015*D26</f>
+      <c r="S26" s="3">
+        <f t="shared" ref="S26:S30" si="24">0.015*D26</f>
         <v>105</v>
       </c>
-      <c r="R26" s="3" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S26" s="3">
-        <v>40</v>
-      </c>
-      <c r="T26" s="3">
+      <c r="T26" s="3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="U26" s="3">
+        <v>40</v>
+      </c>
+      <c r="V26" s="3">
         <v>3</v>
       </c>
-      <c r="U26" s="3">
+      <c r="W26" s="3">
         <v>2018</v>
       </c>
-      <c r="V26" s="4">
-        <f>(AE26+AE27)/2</f>
+      <c r="X26" s="4">
+        <f>(AG26+AG27)/2</f>
         <v>38436</v>
       </c>
-      <c r="W26" s="4">
-        <f>($AH$26+$AH$27)/2</f>
+      <c r="Y26" s="4">
+        <f>($AJ$26+$AJ$27)/2</f>
         <v>27294</v>
       </c>
-      <c r="X26" s="5">
-        <f>V26+MAX(F26*12-2*801,0)</f>
+      <c r="Z26" s="5">
+        <f>X26+MAX(F26*12-2*801,0)</f>
         <v>39834</v>
       </c>
-      <c r="Y26" s="4">
-        <f>W26+MAX(F26*12-2*801,0)</f>
+      <c r="AA26" s="4">
+        <f>Y26+MAX(F26*12-2*801,0)</f>
         <v>28692</v>
       </c>
-      <c r="Z26" s="3"/>
-      <c r="AA26" s="3">
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3">
         <f t="shared" si="14"/>
         <v>12371</v>
       </c>
-      <c r="AB26" s="3">
+      <c r="AD26" s="3">
         <f t="shared" si="16"/>
         <v>83000</v>
       </c>
-      <c r="AC26">
+      <c r="AE26">
         <f>7428/2*3</f>
         <v>11142</v>
       </c>
-      <c r="AD26" s="3">
+      <c r="AF26" s="3">
         <f t="shared" si="5"/>
         <v>7711</v>
       </c>
-      <c r="AE26">
-        <f>AB26-AA26-36-570</f>
+      <c r="AG26">
+        <f>AD26-AC26-36-570</f>
         <v>70023</v>
       </c>
-      <c r="AF26">
-        <f>AE26-AE27</f>
+      <c r="AH26">
+        <f>AG26-AG27</f>
         <v>63174</v>
       </c>
-      <c r="AH26">
-        <f>AE26-(AC26-AG27)</f>
+      <c r="AJ26">
+        <f>AG26-(AE26-AI27)</f>
         <v>54588</v>
       </c>
-      <c r="AJ26" s="3"/>
+      <c r="AL26" s="3"/>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>33</v>
       </c>
@@ -3204,98 +3391,105 @@
         <v>2043</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <f>(N27=FALSE)*40+(N27=TRUE)</f>
+        <v>40</v>
       </c>
       <c r="J27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="K27" t="b">
+      <c r="M27" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="L27" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
+      <c r="N27" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
         <f>0.093*$D27</f>
         <v>74.400000000000006</v>
       </c>
-      <c r="O27">
+      <c r="Q27">
         <f t="shared" si="22"/>
         <v>16</v>
       </c>
-      <c r="P27">
+      <c r="R27">
         <f t="shared" si="23"/>
         <v>64</v>
       </c>
-      <c r="Q27">
+      <c r="S27">
         <f t="shared" si="24"/>
         <v>12</v>
       </c>
-      <c r="R27" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S27">
-        <v>40</v>
-      </c>
-      <c r="T27">
+      <c r="T27" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>40</v>
+      </c>
+      <c r="V27">
         <v>3</v>
       </c>
-      <c r="U27">
+      <c r="W27">
         <v>2018</v>
       </c>
-      <c r="V27" s="4">
-        <f>(AE27+AE26)/2</f>
+      <c r="X27" s="4">
+        <f>(AG27+AG26)/2</f>
         <v>38436</v>
       </c>
-      <c r="W27" s="4">
-        <f>($AH$26+$AH$27)/2</f>
+      <c r="Y27" s="4">
+        <f>($AJ$26+$AJ$27)/2</f>
         <v>27294</v>
       </c>
-      <c r="X27" s="1">
-        <f>V27+MAX(F27*12-2*801,0)</f>
+      <c r="Z27" s="1">
+        <f>X27+MAX(F27*12-2*801,0)</f>
         <v>39834</v>
       </c>
-      <c r="Y27" s="4">
-        <f>W27+MAX(F26*12-2*801,0)</f>
+      <c r="AA27" s="4">
+        <f>Y27+MAX(F26*12-2*801,0)</f>
         <v>28692</v>
       </c>
-      <c r="AA27">
+      <c r="AC27">
         <f t="shared" si="14"/>
         <v>1715</v>
       </c>
-      <c r="AB27">
+      <c r="AD27">
         <f t="shared" si="16"/>
         <v>8600</v>
       </c>
-      <c r="AC27">
+      <c r="AE27">
         <f>7428/2*3</f>
         <v>11142</v>
       </c>
-      <c r="AD27">
+      <c r="AF27">
         <f t="shared" si="5"/>
         <v>1073</v>
       </c>
-      <c r="AE27">
-        <f>AB27-AA27-36</f>
+      <c r="AG27">
+        <f>AD27-AC27-36</f>
         <v>6849</v>
       </c>
-      <c r="AG27">
-        <f>AE27-AC27</f>
+      <c r="AI27">
+        <f>AG27-AE27</f>
         <v>-4293</v>
       </c>
-      <c r="AH27">
-        <f>AE27-(AC27+AG27)</f>
+      <c r="AJ27">
+        <f>AG27-(AE27+AI27)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>33</v>
       </c>
@@ -3318,80 +3512,87 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <f t="shared" ref="H28:H30" si="25">U28+(65-S28)</f>
+        <f t="shared" ref="H28:H30" si="25">W28+(65-U28)</f>
         <v>2068</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <f>(N28=FALSE)*40+(N28=TRUE)</f>
+        <v>1</v>
       </c>
       <c r="J28" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="K28" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K28">
         <v>0</v>
       </c>
       <c r="L28" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28">
+      <c r="M28" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N28" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="O28">
+      <c r="Q28">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="P28">
+      <c r="R28">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="Q28">
+      <c r="S28">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="R28" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S28">
+      <c r="T28" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="U28">
         <v>15</v>
       </c>
-      <c r="T28">
+      <c r="V28">
         <v>3</v>
       </c>
-      <c r="U28">
+      <c r="W28">
         <v>2018</v>
       </c>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
-      <c r="AA28">
-        <f t="shared" ref="AA28:AA30" si="26">(12*D28+(12*B28 - 1000)*(B28&gt;450))</f>
-        <v>0</v>
-      </c>
-      <c r="AB28">
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28">
+        <f t="shared" ref="AC28:AC30" si="26">(12*D28+(12*B28 - 1000)*(B28&gt;450))</f>
+        <v>0</v>
+      </c>
+      <c r="AD28">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AC28">
-        <v>0</v>
-      </c>
-      <c r="AD28">
-        <f t="shared" ref="AD28:AD30" si="27">INT(MAX(12 *(0.96*P28+Q28), MIN(12 *(0.96*P28+Q28+O28),  1900)  ))</f>
-        <v>0</v>
-      </c>
       <c r="AE28">
         <v>0</v>
       </c>
+      <c r="AF28">
+        <f t="shared" ref="AF28:AF30" si="27">INT(MAX(12 *(0.96*R28+S28), MIN(12 *(0.96*R28+S28+Q28),  1900)  ))</f>
+        <v>0</v>
+      </c>
+      <c r="AG28">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>33</v>
       </c>
@@ -3418,76 +3619,83 @@
         <v>2073</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <f>(N29=FALSE)*40+(N29=TRUE)</f>
+        <v>1</v>
       </c>
       <c r="J29" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="K29" t="b">
-        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K29">
         <v>0</v>
       </c>
       <c r="L29" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-      <c r="N29">
+      <c r="M29" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N29" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="O29">
+      <c r="Q29">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="P29">
+      <c r="R29">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="Q29">
+      <c r="S29">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="R29" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S29">
+      <c r="T29" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="U29">
         <v>10</v>
       </c>
-      <c r="T29">
+      <c r="V29">
         <v>3</v>
       </c>
-      <c r="U29">
+      <c r="W29">
         <v>2018</v>
       </c>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
-      <c r="AA29">
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="AB29">
+      <c r="AD29">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AC29">
-        <v>0</v>
-      </c>
-      <c r="AD29">
+      <c r="AE29">
+        <v>0</v>
+      </c>
+      <c r="AF29">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="AE29">
+      <c r="AG29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>33</v>
       </c>
@@ -3514,71 +3722,78 @@
         <v>2075</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <f>(N30=FALSE)*40+(N30=TRUE)</f>
+        <v>1</v>
       </c>
       <c r="J30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="K30" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="L30" t="b">
-        <v>1</v>
-      </c>
-      <c r="M30">
-        <v>0</v>
-      </c>
-      <c r="N30">
+      <c r="M30" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N30" t="b">
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="O30">
+      <c r="Q30">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="P30">
+      <c r="R30">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="Q30">
+      <c r="S30">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="R30" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="S30">
+      <c r="T30" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="U30">
         <v>8</v>
       </c>
-      <c r="T30">
+      <c r="V30">
         <v>3</v>
       </c>
-      <c r="U30">
+      <c r="W30">
         <v>2018</v>
       </c>
-      <c r="W30" s="1"/>
-      <c r="X30" s="1"/>
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
-      <c r="AA30">
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="AB30">
+      <c r="AD30">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AC30">
-        <v>0</v>
-      </c>
-      <c r="AD30">
+      <c r="AE30">
+        <v>0</v>
+      </c>
+      <c r="AF30">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="AE30">
+      <c r="AG30">
         <v>0</v>
       </c>
     </row>

</xml_diff>